<commit_message>
Code with article update
</commit_message>
<xml_diff>
--- a/MusicChannelData.xlsx
+++ b/MusicChannelData.xlsx
@@ -49,173 +49,52 @@
     <t>Keywords</t>
   </si>
   <si>
+    <t>Ru's Piano Ru味春捲</t>
+  </si>
+  <si>
+    <t>kobasolo</t>
+  </si>
+  <si>
+    <t>2CELLOS</t>
+  </si>
+  <si>
+    <t>THE FIRST TAKE</t>
+  </si>
+  <si>
+    <t>あいみょん</t>
+  </si>
+  <si>
+    <t>星野源</t>
+  </si>
+  <si>
+    <t>Ayase / YOASOBI</t>
+  </si>
+  <si>
+    <t>Eric周興哲</t>
+  </si>
+  <si>
+    <t>Ado</t>
+  </si>
+  <si>
+    <t>Joe Hisaishi Official</t>
+  </si>
+  <si>
+    <t>The Piano Guys</t>
+  </si>
+  <si>
+    <t>Pan Piano</t>
+  </si>
+  <si>
+    <t>ヨルシカ / n-buna Official</t>
+  </si>
+  <si>
     <t>美波</t>
   </si>
   <si>
-    <t>2CELLOS</t>
-  </si>
-  <si>
-    <t>ヨルシカ / n-buna Official</t>
-  </si>
-  <si>
-    <t>あいみょん</t>
-  </si>
-  <si>
-    <t>Pan Piano</t>
-  </si>
-  <si>
-    <t>Ado</t>
-  </si>
-  <si>
-    <t>星野源</t>
-  </si>
-  <si>
-    <t>kobasolo</t>
-  </si>
-  <si>
-    <t>Eric周興哲</t>
-  </si>
-  <si>
     <t>周杰倫 Jay Chou</t>
   </si>
   <si>
-    <t>THE FIRST TAKE</t>
-  </si>
-  <si>
-    <t>The Piano Guys</t>
-  </si>
-  <si>
-    <t>Ayase / YOASOBI</t>
-  </si>
-  <si>
-    <t>Joe Hisaishi Official</t>
-  </si>
-  <si>
     <t>First To Eleven</t>
-  </si>
-  <si>
-    <t>Ru's Piano Ru味春捲</t>
-  </si>
-  <si>
-    <t>【美波 Official Youtube Channel】</t>
-  </si>
-  <si>
-    <t>The official home of 2CELLOS - we post our new videos and live concert footage here every few weeks, so keep coming back for the latest 2CELLOS!!</t>
-  </si>
-  <si>
-    <t>ヨルシカ / n-buna official channel</t>
-  </si>
-  <si>
-    <t>兵庫県西宮出身のシンガーソングライター。_x000D_
-15年3月にタワレコ限定single「貴方解剖純愛歌～死ね～」でインディーズデビュー。_x000D_
-16年11月30日、ワーナーミュージック・ジャパン内レーベル unBORDE より1st single「生きていたんだよな」でメジャーデビュー。_x000D_
-17年9月に3枚のシングルを含む1st full album「青春のエキサイトメント」を発表。_x000D_
-8月に5th single「マリーゴールド」をリリース。年末には紅白歌合戦に初出演を果たす。_x000D_
-19年2月にセカンドフルアルバム「瞬間的シックスセンス」を発表。2月18日に初の単独日本武道館公演「AIMYON BUDOKAN -1995-」を開催する。_x000D_
-4月に「「映画クレヨンしんちゃん新婚旅行ハリケーン～失われたひろし～」主題歌を収録したシングル「ハルノヒ」をリリース。_x000D_
-5thシングル「マリーゴールド」が日本国内アーティストでは初の単曲でのストリーミング再生数1億回を突破した。
-7月にTBS系 火曜ドラマ「Heaven？～ご苦楽レストラン～」主題歌「真夏の夜の匂いがする」、10月に映画『空の青さを知る人よ』主題歌2曲を収録したシングル「空の青さを知る人よ」をリリース。_x000D_
-10月から20年の2月までホールとアリーナでの過去最大規模のワンマン・ツアー「AIMYON TOUR 2019 -SIXTH SENSE STORY-」を開催。全箇所即日ソールドアウト。12月には「Billboard 2019年年間TOP ARTISTS」を獲得、「オリコン年間ストリーミングランキング 2019」でも1位を記録し”2019年 1番聴かれたアーティスト”_x000D_
-となった。_x000D_
-日本テレビ「news zero」の1月からの新テーマ曲して書き下ろした楽曲、「さよならの今日に」を配信限定で2月14日にリリース。_x000D_
-4月からOA中の「ハルノヒ」と「マリーゴールド」が起用されたキリンの発泡酒「淡麗グリーンラベル」のTVCMに出演。_x000D_
-6月17日、TBS系 火曜ドラマ『私の家政夫ナギサさん』の主題歌で初のバラードシングル「裸の心」をリリース。_x000D_9月9日に3枚目のフルアルバム「おいしいパスタがあると聞いて」の発表する。</t>
-  </si>
-  <si>
-    <t>台湾のピアニストです！ 
-アニソンを弾いてます～ 
-良かったら、チャンネル登録お願いします（ベルマークもクリックしましょう！）
-宜しくお願いいたします！
-Welcome to my channel~~
-I make piano covers of  Anime/GAME!
-Please subscribe to my channel and click the bell icon to get new video updates!!
-I am so glad to see new SUB :)
-歡迎來到Pan Piano 小P的音樂工房！
-這邊不定期分享動漫鋼琴演奏！歡迎訂閱與按下旁邊的鈴鐺：）
-官方網站 Offical Website：
-小P的音樂工房http://panpiano.com/ 
-～分享動漫鋼琴演奏與教學～</t>
-  </si>
-  <si>
-    <t>元気です。</t>
-  </si>
-  <si>
-    <t>音楽家・俳優・文筆家。
-2010年に1stアルバム『ばかのうた』にてソロデビュー。2016年10月にリリースしたシングル『恋』は、自身も出演したドラマ『逃げるは恥だが役に立つ』の主題歌として社会現象とも呼べる大ヒットを記録した。
-2018年は国民的アニメ映画「映画ドラえもん のび太の宝島」の主題歌、挿入歌を担当。
-そして、2018年12月にリリースしたアルバム『POP VIRUS』は、オリコン週間アルバムランキング、Billboard Japan Hot Albumsにおいて4週連続1位を獲得し、現在も大ヒットを記録中。
-2019年2月から、自身初となる5大ドームツアー“星野源 DOME TOUR 2019『POP VIRUS』”を開催、日本人男性ソロアーティストとして5人目の快挙となる同ツアー全8公演のチケットはすべて即日完売、計33万人を動員した。3月10日の福岡 ヤフオク! ドーム公演を最後に、大盛況ののち全公演を終了した。
-11月からは「Gen Hoshino POP VIRUS World Tour」と題し、ワールド・ツアーの開催も決定。11月23日の上海での公演を皮切りに、ニューヨーク、横浜、台北の4都市で計5公演を行う。</t>
-  </si>
-  <si>
-    <t>毎週金曜19時更新!!音楽プロデューサー、ミュージシャンとして活動するコバソロが贈るエンターテイメントチャンネル!
-楽曲制作、タイアップ等も承っています。
-【コバソロ】
-　演奏、作詞作曲、編曲、撮影、動画作成、各デザインなどすべて自身で手がけるマルチクリエイター。
-「コバソロ」と検索すると自分しか出ないので名前がこれに決定。
-　ライブ、YOUTUBE動画などで活動中!
-無所属
-I live in Japan and I make music.Everything you see + hear on my page was produced and put together by me.
-Also - I absolutely love hearing feedback from you guys.. so please subscribe and leave a comment!</t>
-  </si>
-  <si>
-    <t>Hi! 我是Eric周興哲,
-從前的我 喜歡練習獨立 和鋼琴說話
-現在的自己 
-把鋼琴和說話 變成一種溝通的方式...
-音樂 讓說話變得更自由</t>
-  </si>
-  <si>
-    <t>Jay Chou 周杰倫
-“New King of Asian Pop” — Time magazine (2003)
-“One of the most inﬂuential ﬁgures in Asia”— CNN (2009)
-Music Career
--Iconic musician of the 21st century
--Since his debut in 2000, he has composed, produced, released 14 studio albums, which sold over 30 million copies.
--He holds the highest record sales for Asian male singer, and has won numerous music awards, including 15 GMAs (Chinese Grammy)
-Concerts
--Accomplished 7 world tours, over 300 concerts, performed to more than 10 million people. Jay Chou is celebrating his two decades in the entertainment industry by launching his 20th Anniversary "Carnival " World Tour in Oct. 2019.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A microphone and a white studio.
-And 1 rule.
-You’ve got 1 TAKE.
-Perform anything you like.
-Show us everything you’ve got for that 1 moment.
-ONE TAKE ONLY, ONE LIFE ONLY.
-THE FIRST TAKE
-■「THE FIRST TAKE」OFFICIAL SITE: https://www.thefirsttake.jp/
-■「THE FIRST TAKE」 SNS 
-Instagram： https://www.instagram.com/the_firsttake/
-Twitter： https://twitter.com/The_FirstTake
-Tik Tok： https://vt.tiktok.com/ZSJPuQjcF/
-白いスタジオに置かれた、一本のマイク。
-ここでのルールは、ただ一つ。
-一発撮りのパフォーマンスをすること。
-それ以外は、何をしてもいい。
-一度きりのテイクで、何をみせてくれるだろうか。
-一瞬に込められた想いを見逃すな。
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome to the official The Piano Guys YouTube channel! Paul, a Yamaha dealer who dabbled in videography, Jon, a professional pianist, Al, a music producer and studio engineer, and Steve, a cellist with a creative superpower called ADHD, all serendipitously joined forces to create the most successful YouTube instrumental music group in history. The Piano Guys’ mission is to inspire and spread hope through incomparably imaginative piano music videos filmed all over the world. On this channel you can regularly find piano covers of music from genres like top 40, pop, classic rock, R&amp;B, hip hop, country, and more. Make sure to subscribe and enable all post notifications. For instant updates, check out The Piano Guys via their social media accounts linked below.
-New music coming soon 🎹🎻
-Text us! (801) 217-9512 📱
-</t>
-  </si>
-  <si>
-    <t>シンガーソングライター、ボカロPのAyase、そしてAyaseがコンポーザーを務めるユニット・YOASOBIのYouTubeチャンネルです。</t>
-  </si>
-  <si>
-    <t>久石譲のYouTube公式チャンネルです。Official YouTube channel of Joe Hisaishi.
-Joe Hisaishi—hailed by Pitchfork as “the most acclaimed Japanese composer to have ever worked in film”—has won countless awards for his achievements in composition and film scoring. He is the 8-time winner of the Japanese Academy Award for Best Music; he was awarded the Japan Medal of Honour award in 2009; and he has composed soundtracks for 2 Academy Award-winning films, “Departures” (2008) and “Spirited Away” (2002).
-Hisaishi’s body of work, comprised of nearly 100 film scores and solo albums, draws inspiration from the canon of American minimalist compositions, experimental electronic music, and European and Japanese classical music. He has scored all but one of Hayao Miyazaki’s Studio Ghibli films, including 3 of the top 5 highest-grossing anime films (worldwide).
-Hisaishi, the celebrated Japanese composer known for his beloved film scores and his work with acclaimed filmmakers Hayao
-運営：株式会社ワンダーシティ　©Wonder City Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First to Eleven, Andie Case &amp; Brooke Surgener are coming to Detroit, Chicago, and Cleveland at the end of April! Buy tickets here: www.linktree.com/firsttoeleven
-</t>
   </si>
   <si>
     <t>I’m RuRu, a piano youtuber from Taiwan.
@@ -243,172 +122,293 @@
 🎹合作洽談/Business：rurupianomusic@gmail.com</t>
   </si>
   <si>
+    <t>毎週金曜19時更新!!音楽プロデューサー、ミュージシャンとして活動するコバソロが贈るエンターテイメントチャンネル!
+楽曲制作、タイアップ等も承っています。
+【コバソロ】
+　演奏、作詞作曲、編曲、撮影、動画作成、各デザインなどすべて自身で手がけるマルチクリエイター。
+「コバソロ」と検索すると自分しか出ないので名前がこれに決定。
+　ライブ、YOUTUBE動画などで活動中!
+無所属
+I live in Japan and I make music.Everything you see + hear on my page was produced and put together by me.
+Also - I absolutely love hearing feedback from you guys.. so please subscribe and leave a comment!</t>
+  </si>
+  <si>
+    <t>The official home of 2CELLOS - we post our new videos and live concert footage here every few weeks, so keep coming back for the latest 2CELLOS!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A microphone and a white studio.
+And 1 rule.
+You’ve got 1 TAKE.
+Perform anything you like.
+Show us everything you’ve got for that 1 moment.
+ONE TAKE ONLY, ONE LIFE ONLY.
+THE FIRST TAKE
+■「THE FIRST TAKE」OFFICIAL SITE: https://www.thefirsttake.jp/
+■「THE FIRST TAKE」 SNS 
+Instagram： https://www.instagram.com/the_firsttake/
+Twitter： https://twitter.com/The_FirstTake
+Tik Tok： https://vt.tiktok.com/ZSJPuQjcF/
+白いスタジオに置かれた、一本のマイク。
+ここでのルールは、ただ一つ。
+一発撮りのパフォーマンスをすること。
+それ以外は、何をしてもいい。
+一度きりのテイクで、何をみせてくれるだろうか。
+一瞬に込められた想いを見逃すな。
+</t>
+  </si>
+  <si>
+    <t>兵庫県西宮出身のシンガーソングライター。_x000D_
+15年3月にタワレコ限定single「貴方解剖純愛歌～死ね～」でインディーズデビュー。_x000D_
+16年11月30日、ワーナーミュージック・ジャパン内レーベル unBORDE より1st single「生きていたんだよな」でメジャーデビュー。_x000D_
+17年9月に3枚のシングルを含む1st full album「青春のエキサイトメント」を発表。_x000D_
+8月に5th single「マリーゴールド」をリリース。年末には紅白歌合戦に初出演を果たす。_x000D_
+19年2月にセカンドフルアルバム「瞬間的シックスセンス」を発表。2月18日に初の単独日本武道館公演「AIMYON BUDOKAN -1995-」を開催する。_x000D_
+4月に「「映画クレヨンしんちゃん新婚旅行ハリケーン～失われたひろし～」主題歌を収録したシングル「ハルノヒ」をリリース。_x000D_
+5thシングル「マリーゴールド」が日本国内アーティストでは初の単曲でのストリーミング再生数1億回を突破した。
+7月にTBS系 火曜ドラマ「Heaven？～ご苦楽レストラン～」主題歌「真夏の夜の匂いがする」、10月に映画『空の青さを知る人よ』主題歌2曲を収録したシングル「空の青さを知る人よ」をリリース。_x000D_
+10月から20年の2月までホールとアリーナでの過去最大規模のワンマン・ツアー「AIMYON TOUR 2019 -SIXTH SENSE STORY-」を開催。全箇所即日ソールドアウト。12月には「Billboard 2019年年間TOP ARTISTS」を獲得、「オリコン年間ストリーミングランキング 2019」でも1位を記録し”2019年 1番聴かれたアーティスト”_x000D_
+となった。_x000D_
+日本テレビ「news zero」の1月からの新テーマ曲して書き下ろした楽曲、「さよならの今日に」を配信限定で2月14日にリリース。_x000D_
+4月からOA中の「ハルノヒ」と「マリーゴールド」が起用されたキリンの発泡酒「淡麗グリーンラベル」のTVCMに出演。_x000D_
+6月17日、TBS系 火曜ドラマ『私の家政夫ナギサさん』の主題歌で初のバラードシングル「裸の心」をリリース。_x000D_9月9日に3枚目のフルアルバム「おいしいパスタがあると聞いて」の発表する。</t>
+  </si>
+  <si>
+    <t>音楽家・俳優・文筆家。
+2010年に1stアルバム『ばかのうた』にてソロデビュー。2016年10月にリリースしたシングル『恋』は、自身も出演したドラマ『逃げるは恥だが役に立つ』の主題歌として社会現象とも呼べる大ヒットを記録した。
+2018年は国民的アニメ映画「映画ドラえもん のび太の宝島」の主題歌、挿入歌を担当。
+そして、2018年12月にリリースしたアルバム『POP VIRUS』は、オリコン週間アルバムランキング、Billboard Japan Hot Albumsにおいて4週連続1位を獲得し、現在も大ヒットを記録中。
+2019年2月から、自身初となる5大ドームツアー“星野源 DOME TOUR 2019『POP VIRUS』”を開催、日本人男性ソロアーティストとして5人目の快挙となる同ツアー全8公演のチケットはすべて即日完売、計33万人を動員した。3月10日の福岡 ヤフオク! ドーム公演を最後に、大盛況ののち全公演を終了した。
+11月からは「Gen Hoshino POP VIRUS World Tour」と題し、ワールド・ツアーの開催も決定。11月23日の上海での公演を皮切りに、ニューヨーク、横浜、台北の4都市で計5公演を行う。</t>
+  </si>
+  <si>
+    <t>シンガーソングライター、ボカロPのAyase、そしてAyaseがコンポーザーを務めるユニット・YOASOBIのYouTubeチャンネルです。</t>
+  </si>
+  <si>
+    <t>Hi! 我是Eric周興哲,
+從前的我 喜歡練習獨立 和鋼琴說話
+現在的自己 
+把鋼琴和說話 變成一種溝通的方式...
+音樂 讓說話變得更自由</t>
+  </si>
+  <si>
+    <t>元気です。</t>
+  </si>
+  <si>
+    <t>久石譲のYouTube公式チャンネルです。Official YouTube channel of Joe Hisaishi.
+Joe Hisaishi—hailed by Pitchfork as “the most acclaimed Japanese composer to have ever worked in film”—has won countless awards for his achievements in composition and film scoring. He is the 8-time winner of the Japanese Academy Award for Best Music; he was awarded the Japan Medal of Honour award in 2009; and he has composed soundtracks for 2 Academy Award-winning films, “Departures” (2008) and “Spirited Away” (2002).
+Hisaishi’s body of work, comprised of nearly 100 film scores and solo albums, draws inspiration from the canon of American minimalist compositions, experimental electronic music, and European and Japanese classical music. He has scored all but one of Hayao Miyazaki’s Studio Ghibli films, including 3 of the top 5 highest-grossing anime films (worldwide).
+Hisaishi, the celebrated Japanese composer known for his beloved film scores and his work with acclaimed filmmakers Hayao
+運営：株式会社ワンダーシティ　©Wonder City Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the official The Piano Guys YouTube channel! Paul, a Yamaha dealer who dabbled in videography, Jon, a professional pianist, Al, a music producer and studio engineer, and Steve, a cellist with a creative superpower called ADHD, all serendipitously joined forces to create the most successful YouTube instrumental music group in history. The Piano Guys’ mission is to inspire and spread hope through incomparably imaginative piano music videos filmed all over the world. On this channel you can regularly find piano covers of music from genres like top 40, pop, classic rock, R&amp;B, hip hop, country, and more. Make sure to subscribe and enable all post notifications. For instant updates, check out The Piano Guys via their social media accounts linked below.
+New music coming soon 🎹🎻
+Text us! (801) 217-9512 📱
+</t>
+  </si>
+  <si>
+    <t>台湾のピアニストです！ 
+アニソンを弾いてます～ 
+良かったら、チャンネル登録お願いします（ベルマークもクリックしましょう！）
+宜しくお願いいたします！
+Welcome to my channel~~
+I make piano covers of  Anime/GAME!
+Please subscribe to my channel and click the bell icon to get new video updates!!
+I am so glad to see new SUB :)
+歡迎來到Pan Piano 小P的音樂工房！
+這邊不定期分享動漫鋼琴演奏！歡迎訂閱與按下旁邊的鈴鐺：）
+官方網站 Offical Website：
+小P的音樂工房http://panpiano.com/ 
+～分享動漫鋼琴演奏與教學～</t>
+  </si>
+  <si>
+    <t>ヨルシカ / n-buna official channel</t>
+  </si>
+  <si>
+    <t>【美波 Official Youtube Channel】</t>
+  </si>
+  <si>
+    <t>Jay Chou 周杰倫
+“New King of Asian Pop” — Time magazine (2003)
+“One of the most inﬂuential ﬁgures in Asia”— CNN (2009)
+Music Career
+-Iconic musician of the 21st century
+-Since his debut in 2000, he has composed, produced, released 14 studio albums, which sold over 30 million copies.
+-He holds the highest record sales for Asian male singer, and has won numerous music awards, including 15 GMAs (Chinese Grammy)
+Concerts
+-Accomplished 7 world tours, over 300 concerts, performed to more than 10 million people. Jay Chou is celebrating his two decades in the entertainment industry by launching his 20th Anniversary "Carnival " World Tour in Oct. 2019.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First to Eleven, Andie Case &amp; Brooke Surgener are coming to Detroit, Chicago, and Cleveland at the end of April! Buy tickets here: www.linktree.com/firsttoeleven
+</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
     <t>JP</t>
   </si>
   <si>
     <t>HR</t>
   </si>
   <si>
-    <t>TW</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
+    <t>UUAYrMNl92jw6cpjdpBP8JyA</t>
+  </si>
+  <si>
+    <t>UUDbQblY1XASbgqOXmy6FOFQ</t>
+  </si>
+  <si>
+    <t>UUyjuFsbclXyntSRMBAILzbw</t>
+  </si>
+  <si>
+    <t>UU9zY_E8mcAo_Oq772LEZq8Q</t>
+  </si>
+  <si>
+    <t>UUQVhrypJhw1HxuRV4gX6hoQ</t>
+  </si>
+  <si>
+    <t>UUPKlrgZXnnb89nSeITvTdGA</t>
+  </si>
+  <si>
+    <t>UUvpredjG93ifbCP1Y77JyFA</t>
+  </si>
+  <si>
+    <t>UU7S48XRADBqamQbgLxpBFcQ</t>
+  </si>
+  <si>
+    <t>UUln9P4Qm3-EAY4aiEPmRwEA</t>
+  </si>
+  <si>
+    <t>UUxyzciBLt1Hyw06dlqwAIkw</t>
+  </si>
+  <si>
+    <t>UUmKurapML4BF9Bjtj4RbvXw</t>
+  </si>
+  <si>
+    <t>UUI7ktPB6toqucpkkCiolwLg</t>
+  </si>
+  <si>
+    <t>UURIgIJQWuBJ0Cv_VlU3USNA</t>
+  </si>
+  <si>
     <t>UU2JzylaIF8qeowc7-5VwwmA</t>
   </si>
   <si>
-    <t>UUyjuFsbclXyntSRMBAILzbw</t>
-  </si>
-  <si>
-    <t>UURIgIJQWuBJ0Cv_VlU3USNA</t>
-  </si>
-  <si>
-    <t>UUQVhrypJhw1HxuRV4gX6hoQ</t>
-  </si>
-  <si>
-    <t>UUI7ktPB6toqucpkkCiolwLg</t>
-  </si>
-  <si>
-    <t>UUln9P4Qm3-EAY4aiEPmRwEA</t>
-  </si>
-  <si>
-    <t>UUPKlrgZXnnb89nSeITvTdGA</t>
-  </si>
-  <si>
-    <t>UUDbQblY1XASbgqOXmy6FOFQ</t>
-  </si>
-  <si>
-    <t>UU7S48XRADBqamQbgLxpBFcQ</t>
-  </si>
-  <si>
     <t>UU8CU5nVhCQIdAGrFFp4loOQ</t>
   </si>
   <si>
-    <t>UU9zY_E8mcAo_Oq772LEZq8Q</t>
-  </si>
-  <si>
-    <t>UUmKurapML4BF9Bjtj4RbvXw</t>
-  </si>
-  <si>
-    <t>UUvpredjG93ifbCP1Y77JyFA</t>
-  </si>
-  <si>
-    <t>UUxyzciBLt1Hyw06dlqwAIkw</t>
-  </si>
-  <si>
     <t>UUcE10s4MFy4eed7q7QkonZg</t>
   </si>
   <si>
-    <t>UUAYrMNl92jw6cpjdpBP8JyA</t>
-  </si>
-  <si>
-    <t>['Music_of_Asia', 'Pop_music', 'Independent_music', 'Rock_music', 'Music']</t>
-  </si>
-  <si>
-    <t>['Classical_music', 'Independent_music', 'Pop_music', 'Rock_music', 'Music']</t>
-  </si>
-  <si>
-    <t>['Rock_music', 'Independent_music', 'Music_of_Asia', 'Pop_music', 'Music']</t>
-  </si>
-  <si>
-    <t>['Rock_music', 'Music_of_Asia', 'Pop_music', 'Music']</t>
-  </si>
-  <si>
-    <t>['Music_of_Asia', 'Music', 'Classical_music']</t>
-  </si>
-  <si>
-    <t>['Electronic_music', 'Rock_music', 'Independent_music', 'Music_of_Asia', 'Pop_music', 'Music']</t>
-  </si>
-  <si>
-    <t>['Music_of_Asia', 'Music', 'Pop_music']</t>
-  </si>
-  <si>
-    <t>['Classical_music', 'Music', 'Pop_music']</t>
+    <t>['Classical_music', 'Music_of_Asia', 'Music']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Music_of_Asia', 'Music']</t>
+  </si>
+  <si>
+    <t>['Rock_music', 'Classical_music', 'Independent_music', 'Music', 'Pop_music']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Music', 'Music_of_Asia', 'Rock_music']</t>
+  </si>
+  <si>
+    <t>['Music_of_Asia', 'Rock_music', 'Pop_music', 'Music', 'Independent_music', 'Electronic_music']</t>
   </si>
   <si>
     <t>['Classical_music', 'Music']</t>
   </si>
   <si>
-    <t>['Independent_music', 'Pop_music', 'Music', 'Rock_music']</t>
+    <t>['Classical_music', 'Pop_music', 'Music']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Independent_music', 'Rock_music', 'Music_of_Asia', 'Music']</t>
+  </si>
+  <si>
+    <t>['Music_of_Asia', 'Music', 'Independent_music', 'Pop_music', 'Rock_music']</t>
+  </si>
+  <si>
+    <t>['Music', 'Independent_music', 'Rock_music', 'Pop_music']</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu_-ZUJbCF-LRu259pFVkL4zxoEfNcqq2MNmMccjJw=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu-9S3og5Ip2zFASnqMWKkjWatBfPT9ELeqUbTSL1A=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu9V7gXnpIUCJYKKY_KANCGKI-0lrr0VeoRXYVce6A=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu9H0hC1Gt8ZLT4V9Z5342HDhba7YsApb9sa_0EgvQ=s800-c-k-c0x00ffffff-no-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/EuK-WoKwja8NatLUU0SfdSyxhDnlHRSV7tvtkWRDeYuNjsigu5vrMHyBAn5WVakHVWN_hICCvw=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/DLCVX6ArRGaHMe4k4N7Q_QtYiSOwbJ0pHi9zNwegysTq2ozs3G3_CPxImF-2hh0E2SYVGOEc=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu_8o8D8yLIaOLRZMOmVO0fS85nM-VlmWNJHQIJFLQ=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/GFgkrFvg6tIF3XzfGJIb3q722cC-viI_SRplnNx3P5LWsGDtZlXTuxDOOG9WfZxWb1e-Iphy=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/I3ckNVLPQq04aQklOnRctTEnBjf7pkppVLV7WYe4Nb4g3sge1h-2IlXAvLnRGgrMkMfL4NadPQ=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/6pJyAmpgkwyRL5b3JCABfxOkfluyRw8wIaTS0cHMIGhOKr5dEmuquC9nsCxUl8Yp3KGQGavE-g=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/VC8eWCWtSO-5LN-f-IQGDu8HfwmwoZaA9kuIwa7v-o0S0DX0YTVlNvgxErve31v5qeOF9jiSiw=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu8sHT4fM2VGUuzkgMcYjsPHodm0PTpgWZ-14jj87w=s800-c-k-c0x00ffffff-no-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu_b_-qhgW9Ix681w7CVRpJmkqrciDIrCPb3fRjw=s800-c-k-c0x00ffffff-no-rj-mo</t>
   </si>
   <si>
     <t>https://yt3.ggpht.com/ytc/AMLnZu-a_zfDCmdvUihG0DgQdTY6aPT4lQ5Sst5qnvczgg=s800-c-k-c0x00ffffff-no-rj-mo</t>
   </si>
   <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu9V7gXnpIUCJYKKY_KANCGKI-0lrr0VeoRXYVce6A=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_b_-qhgW9Ix681w7CVRpJmkqrciDIrCPb3fRjw=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/EuK-WoKwja8NatLUU0SfdSyxhDnlHRSV7tvtkWRDeYuNjsigu5vrMHyBAn5WVakHVWN_hICCvw=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu8sHT4fM2VGUuzkgMcYjsPHodm0PTpgWZ-14jj87w=s800-c-k-c0x00ffffff-no-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/I3ckNVLPQq04aQklOnRctTEnBjf7pkppVLV7WYe4Nb4g3sge1h-2IlXAvLnRGgrMkMfL4NadPQ=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/DLCVX6ArRGaHMe4k4N7Q_QtYiSOwbJ0pHi9zNwegysTq2ozs3G3_CPxImF-2hh0E2SYVGOEc=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu-9S3og5Ip2zFASnqMWKkjWatBfPT9ELeqUbTSL1A=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/GFgkrFvg6tIF3XzfGJIb3q722cC-viI_SRplnNx3P5LWsGDtZlXTuxDOOG9WfZxWb1e-Iphy=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
     <t>https://yt3.ggpht.com/OvyupgLYH05byQQoYNw6BtXoCw1ygFYTMtGhk0vOTaOii8U9x5NYK1R4JD7FJAUCouqy_8JA=s800-c-k-c0x00ffffff-no-nd-rj</t>
   </si>
   <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu9H0hC1Gt8ZLT4V9Z5342HDhba7YsApb9sa_0EgvQ=s800-c-k-c0x00ffffff-no-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/VC8eWCWtSO-5LN-f-IQGDu8HfwmwoZaA9kuIwa7v-o0S0DX0YTVlNvgxErve31v5qeOF9jiSiw=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_8o8D8yLIaOLRZMOmVO0fS85nM-VlmWNJHQIJFLQ=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/6pJyAmpgkwyRL5b3JCABfxOkfluyRw8wIaTS0cHMIGhOKr5dEmuquC9nsCxUl8Yp3KGQGavE-g=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
     <t>https://yt3.ggpht.com/Xsyf4kJrHNMZl8ZJD-2wSWe_1Ob3s2hNFjQj0QCaJZjBXUZ40ORfoWgIilhxLEz_XR9NM7ogbg=s800-c-k-c0x00ffffff-no-nd-rj</t>
   </si>
   <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_-ZUJbCF-LRu259pFVkL4zxoEfNcqq2MNmMccjJw=s800-c-k-c0x00ffffff-no-rj-mo</t>
+    <t>鋼琴 Ru味春捲 "Ru's Piano" "Ru Piano" Piano ピアノ "Anime Piano" "動漫 鋼琴" Pianist "Piano Cover" RUsPiano 鋼琴女神 "Cosplay Piano" "Cosplay 鋼琴" "ACG ピアノ" ピアノ</t>
+  </si>
+  <si>
+    <t>KOBASOLO コバソロ リトルタートルズ 音楽 music インディーズ little turtles live コバ カメ 癒し new 新宿 ストリート タワーレコード ＰＯＰ Ｒ＆Ｂ ＳＯＵＬ ビデオ</t>
+  </si>
+  <si>
+    <t>2CELLOS Luka Sulic Stjepan Hauser Two Cellos</t>
+  </si>
+  <si>
+    <t>星野源 ほしのげん ホシノゲン "Gen Hoshino" "Hoshino Gen" "星野 源"</t>
+  </si>
+  <si>
+    <t>周興哲</t>
+  </si>
+  <si>
+    <t>アド あぼ ado "アド 歌い手" ADO Ado "Ado TikTok" "アド ティックトック" "Ado 歌い手" 歌い手 "ado 邪魔" エーディーオー エイド うっせぇわ USSEEWA うっせぇわ 会いたくて 踊 レディメイド 夜のピエロ ギラギラ よくばり Ayase</t>
+  </si>
+  <si>
+    <t>thepianoguys "the piano guys" "piano guys" "piano guy" "piano guys youtube" "youtube piano guys" song music cover instrumental cello "cello song" "cello music" "cello cover" "cover cello" "cello instrumental" "instrumental cello" "cello performance" "cello live" "live cello" "cello songs" piano "piano song" "piano music" "piano cover" "cover piano" "piano instrumental" "instrumental piano" "piano performance" "live piano" "piano live" "piano songs" classical "classical music" "classical piano"</t>
+  </si>
+  <si>
+    <t>鋼琴 演奏 ACG 動畫 漫畫 piano ピアノ アニメ 弾いてみた コスプレ パンピアノ "pan piano"</t>
   </si>
   <si>
     <t>シンガーソングライター</t>
   </si>
   <si>
-    <t>2CELLOS Luka Sulic Stjepan Hauser Two Cellos</t>
-  </si>
-  <si>
-    <t>鋼琴 演奏 ACG 動畫 漫畫 piano ピアノ アニメ 弾いてみた コスプレ パンピアノ "pan piano"</t>
-  </si>
-  <si>
-    <t>アド あぼ ado "アド 歌い手" ADO Ado "Ado TikTok" "アド ティックトック" "Ado 歌い手" 歌い手 "ado 邪魔" エーディーオー エイド うっせぇわ USSEEWA うっせぇわ 会いたくて 踊 レディメイド 夜のピエロ ギラギラ よくばり Ayase</t>
-  </si>
-  <si>
-    <t>星野源 ほしのげん ホシノゲン "Gen Hoshino" "Hoshino Gen" "星野 源"</t>
-  </si>
-  <si>
-    <t>KOBASOLO コバソロ リトルタートルズ 音楽 music インディーズ little turtles live コバ カメ 癒し new 新宿 ストリート タワーレコード ＰＯＰ Ｒ＆Ｂ ＳＯＵＬ ビデオ</t>
-  </si>
-  <si>
-    <t>周興哲</t>
-  </si>
-  <si>
-    <t>thepianoguys "the piano guys" "piano guys" "piano guy" "piano guys youtube" "youtube piano guys" song music cover instrumental cello "cello song" "cello music" "cello cover" "cover cello" "cello instrumental" "instrumental cello" "cello performance" "cello live" "live cello" "cello songs" piano "piano song" "piano music" "piano cover" "cover piano" "piano instrumental" "instrumental piano" "piano performance" "live piano" "piano live" "piano songs" classical "classical music" "classical piano"</t>
-  </si>
-  <si>
     <t>"first to eleven" "first to eleven youtube" "youtube first to eleven" f211 "f211 youtube" "youtube f211" female "female vocalist" "female singer" singing music artist "music artist" cover covers "cover band" band rock pop "pop rock" "rock cover" "pop cover" "pop rock cover"</t>
-  </si>
-  <si>
-    <t>鋼琴 Ru味春捲 "Ru's Piano" "Ru Piano" Piano ピアノ "Anime Piano" "動漫 鋼琴" Pianist "Piano Cover" RUsPiano 鋼琴女神 "Cosplay Piano" "Cosplay 鋼琴" "ACG ピアノ" ピアノ</t>
   </si>
 </sst>
 </file>
@@ -835,22 +835,22 @@
         <v>27</v>
       </c>
       <c r="D2" s="2">
-        <v>42372</v>
+        <v>43173</v>
       </c>
       <c r="E2" t="s">
         <v>43</v>
       </c>
       <c r="F2">
-        <v>1310000</v>
+        <v>2310000</v>
       </c>
       <c r="G2">
-        <v>414259547</v>
+        <v>299852235</v>
       </c>
       <c r="H2" t="s">
         <v>47</v>
       </c>
       <c r="I2">
-        <v>7</v>
+        <v>405</v>
       </c>
       <c r="J2" t="s">
         <v>63</v>
@@ -873,22 +873,22 @@
         <v>28</v>
       </c>
       <c r="D3" s="2">
-        <v>40833</v>
+        <v>39629</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
       </c>
       <c r="F3">
-        <v>6290000</v>
+        <v>3010000</v>
       </c>
       <c r="G3">
-        <v>1617515031</v>
+        <v>1428323212</v>
       </c>
       <c r="H3" t="s">
         <v>48</v>
       </c>
       <c r="I3">
-        <v>213</v>
+        <v>500</v>
       </c>
       <c r="J3" t="s">
         <v>64</v>
@@ -911,25 +911,31 @@
         <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>41355</v>
+        <v>40833</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
       </c>
       <c r="F4">
-        <v>2560000</v>
+        <v>6300000</v>
       </c>
       <c r="G4">
-        <v>1432961356</v>
+        <v>1623449197</v>
       </c>
       <c r="H4" t="s">
         <v>49</v>
       </c>
       <c r="I4">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="J4" t="s">
         <v>65</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>75</v>
+      </c>
+      <c r="L4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -943,28 +949,28 @@
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>41712</v>
+        <v>43774</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
       </c>
       <c r="F5">
-        <v>1750000</v>
+        <v>6860000</v>
       </c>
       <c r="G5">
-        <v>1529961777</v>
+        <v>2455470515</v>
       </c>
       <c r="H5" t="s">
         <v>50</v>
       </c>
       <c r="I5">
-        <v>24</v>
+        <v>435</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -978,31 +984,28 @@
         <v>31</v>
       </c>
       <c r="D6" s="2">
-        <v>42578</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
+        <v>41712</v>
       </c>
       <c r="F6">
-        <v>3360000</v>
+        <v>1760000</v>
       </c>
       <c r="G6">
-        <v>527595749</v>
+        <v>1540391747</v>
       </c>
       <c r="H6" t="s">
         <v>51</v>
       </c>
       <c r="I6">
-        <v>552</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>77</v>
       </c>
       <c r="L6" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1016,25 +1019,25 @@
         <v>32</v>
       </c>
       <c r="D7" s="2">
-        <v>43330</v>
+        <v>42132</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F7">
-        <v>4130000</v>
+        <v>1470000</v>
       </c>
       <c r="G7">
-        <v>1469750934</v>
+        <v>932112708</v>
       </c>
       <c r="H7" t="s">
         <v>52</v>
       </c>
       <c r="I7">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>78</v>
@@ -1054,31 +1057,28 @@
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>42132</v>
+        <v>43420</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8">
-        <v>1470000</v>
+        <v>4070000</v>
       </c>
       <c r="G8">
-        <v>926627202</v>
+        <v>2091104911</v>
       </c>
       <c r="H8" t="s">
         <v>53</v>
       </c>
       <c r="I8">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="L8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1092,31 +1092,31 @@
         <v>34</v>
       </c>
       <c r="D9" s="2">
-        <v>39629</v>
+        <v>41855</v>
       </c>
       <c r="E9" t="s">
         <v>43</v>
       </c>
       <c r="F9">
-        <v>3010000</v>
+        <v>1110000</v>
       </c>
       <c r="G9">
-        <v>1423840904</v>
+        <v>1287840309</v>
       </c>
       <c r="H9" t="s">
         <v>54</v>
       </c>
       <c r="I9">
-        <v>499</v>
+        <v>131</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1130,31 +1130,31 @@
         <v>35</v>
       </c>
       <c r="D10" s="2">
-        <v>41855</v>
+        <v>43330</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10">
-        <v>1100000</v>
+        <v>4220000</v>
       </c>
       <c r="G10">
-        <v>1277060624</v>
+        <v>1534485518</v>
       </c>
       <c r="H10" t="s">
         <v>55</v>
       </c>
       <c r="I10">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>81</v>
       </c>
       <c r="L10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1168,25 +1168,25 @@
         <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>43767</v>
+        <v>42762</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11">
-        <v>2670000</v>
+        <v>876000</v>
       </c>
       <c r="G11">
-        <v>3403847506</v>
+        <v>137620621</v>
       </c>
       <c r="H11" t="s">
         <v>56</v>
       </c>
       <c r="I11">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="J11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>82</v>
@@ -1203,28 +1203,31 @@
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>43774</v>
+        <v>39532</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F12">
-        <v>6810000</v>
+        <v>7030000</v>
       </c>
       <c r="G12">
-        <v>2417822321</v>
+        <v>2214772684</v>
       </c>
       <c r="H12" t="s">
         <v>57</v>
       </c>
       <c r="I12">
-        <v>430</v>
+        <v>132</v>
       </c>
       <c r="J12" t="s">
         <v>69</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>83</v>
+      </c>
+      <c r="L12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1238,25 +1241,25 @@
         <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>39532</v>
+        <v>42578</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F13">
-        <v>7030000</v>
+        <v>3400000</v>
       </c>
       <c r="G13">
-        <v>2209994362</v>
+        <v>532432474</v>
       </c>
       <c r="H13" t="s">
         <v>58</v>
       </c>
       <c r="I13">
-        <v>131</v>
+        <v>557</v>
       </c>
       <c r="J13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>84</v>
@@ -1276,25 +1279,22 @@
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>43420</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
+        <v>41355</v>
       </c>
       <c r="F14">
-        <v>4020000</v>
+        <v>2570000</v>
       </c>
       <c r="G14">
-        <v>2054383268</v>
+        <v>1446571523</v>
       </c>
       <c r="H14" t="s">
         <v>59</v>
       </c>
       <c r="I14">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="J14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>85</v>
@@ -1311,28 +1311,31 @@
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>42762</v>
+        <v>42372</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F15">
-        <v>871000</v>
+        <v>1310000</v>
       </c>
       <c r="G15">
-        <v>135036332</v>
+        <v>417607213</v>
       </c>
       <c r="H15" t="s">
         <v>60</v>
       </c>
       <c r="I15">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="J15" t="s">
         <v>71</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>86</v>
+      </c>
+      <c r="L15" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1346,31 +1349,28 @@
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>42346</v>
+        <v>43767</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F16">
-        <v>1450000</v>
+        <v>2680000</v>
       </c>
       <c r="G16">
-        <v>417419802</v>
+        <v>3428410144</v>
       </c>
       <c r="H16" t="s">
         <v>61</v>
       </c>
       <c r="I16">
-        <v>311</v>
+        <v>21</v>
       </c>
       <c r="J16" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="L16" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1384,25 +1384,25 @@
         <v>42</v>
       </c>
       <c r="D17" s="2">
-        <v>43173</v>
+        <v>42346</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17">
-        <v>2280000</v>
+        <v>1450000</v>
       </c>
       <c r="G17">
-        <v>295168239</v>
+        <v>421481683</v>
       </c>
       <c r="H17" t="s">
         <v>62</v>
       </c>
       <c r="I17">
-        <v>401</v>
+        <v>314</v>
       </c>
       <c r="J17" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
All music channel file are updated
</commit_message>
<xml_diff>
--- a/MusicChannelData.xlsx
+++ b/MusicChannelData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="101">
   <si>
     <t>ChannelTitle</t>
   </si>
@@ -49,171 +49,61 @@
     <t>Keywords</t>
   </si>
   <si>
+    <t>Ru's Piano Ru味春捲</t>
+  </si>
+  <si>
+    <t>Eric周興哲</t>
+  </si>
+  <si>
+    <t>星野源</t>
+  </si>
+  <si>
+    <t>kobasolo</t>
+  </si>
+  <si>
+    <t>Pan Piano</t>
+  </si>
+  <si>
+    <t>First To Eleven</t>
+  </si>
+  <si>
+    <t>あいみょん</t>
+  </si>
+  <si>
+    <t>The Piano Guys</t>
+  </si>
+  <si>
+    <t>Ado</t>
+  </si>
+  <si>
+    <t>Joe Hisaishi Official</t>
+  </si>
+  <si>
+    <t>Ayase / YOASOBI</t>
+  </si>
+  <si>
     <t>ヨルシカ / n-buna Official</t>
   </si>
   <si>
-    <t>kobasolo</t>
+    <t>周杰倫 Jay Chou</t>
+  </si>
+  <si>
+    <t>美波</t>
   </si>
   <si>
     <t>THE FIRST TAKE</t>
   </si>
   <si>
-    <t>周杰倫 Jay Chou</t>
-  </si>
-  <si>
-    <t>Pan Piano</t>
-  </si>
-  <si>
     <t>2CELLOS</t>
   </si>
   <si>
-    <t>Joe Hisaishi Official</t>
-  </si>
-  <si>
-    <t>First To Eleven</t>
-  </si>
-  <si>
-    <t>Ado</t>
-  </si>
-  <si>
-    <t>The Piano Guys</t>
-  </si>
-  <si>
-    <t>Eric周興哲</t>
-  </si>
-  <si>
-    <t>美波</t>
-  </si>
-  <si>
-    <t>あいみょん</t>
-  </si>
-  <si>
-    <t>Ru's Piano Ru味春捲</t>
-  </si>
-  <si>
-    <t>Ayase / YOASOBI</t>
-  </si>
-  <si>
-    <t>星野源</t>
-  </si>
-  <si>
-    <t>ヨルシカ / n-buna official channel</t>
-  </si>
-  <si>
-    <t>毎週金曜19時更新!!音楽プロデューサー、ミュージシャンとして活動するコバソロが贈るエンターテイメントチャンネル!
-楽曲制作、タイアップ等も承っています。
-【コバソロ】
-　演奏、作詞作曲、編曲、撮影、動画作成、各デザインなどすべて自身で手がけるマルチクリエイター。
-「コバソロ」と検索すると自分しか出ないので名前がこれに決定。
-　ライブ、YOUTUBE動画などで活動中!
-無所属
-I live in Japan and I make music.Everything you see + hear on my page was produced and put together by me.
-Also - I absolutely love hearing feedback from you guys.. so please subscribe and leave a comment!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A microphone and a white studio.
-And 1 rule.
-You’ve got 1 TAKE.
-Perform anything you like.
-Show us everything you’ve got for that 1 moment.
-ONE TAKE ONLY, ONE LIFE ONLY.
-THE FIRST TAKE
-■「THE FIRST TAKE」OFFICIAL SITE: https://www.thefirsttake.jp/
-■「THE FIRST TAKE」 SNS 
-Instagram： https://www.instagram.com/the_firsttake/
-Twitter： https://twitter.com/The_FirstTake
-Tik Tok： https://vt.tiktok.com/ZSJPuQjcF/
-白いスタジオに置かれた、一本のマイク。
-ここでのルールは、ただ一つ。
-一発撮りのパフォーマンスをすること。
-それ以外は、何をしてもいい。
-一度きりのテイクで、何をみせてくれるだろうか。
-一瞬に込められた想いを見逃すな。
-</t>
-  </si>
-  <si>
-    <t>Jay Chou 周杰倫
-“New King of Asian Pop” — Time magazine (2003)
-“One of the most inﬂuential ﬁgures in Asia”— CNN (2009)
-Music Career
--Iconic musician of the 21st century
--Since his debut in 2000, he has composed, produced, released 14 studio albums, which sold over 30 million copies.
--He holds the highest record sales for Asian male singer, and has won numerous music awards, including 15 GMAs (Chinese Grammy)
-Concerts
--Accomplished 7 world tours, over 300 concerts, performed to more than 10 million people. Jay Chou is celebrating his two decades in the entertainment industry by launching his 20th Anniversary "Carnival " World Tour in Oct. 2019.</t>
-  </si>
-  <si>
-    <t>台湾のピアニストです！ 
-アニソンを弾いてます～ 
-良かったら、チャンネル登録お願いします（ベルマークもクリックしましょう！）
-宜しくお願いいたします！
-Welcome to my channel~~
-I make piano covers of  Anime/GAME!
-Please subscribe to my channel and click the bell icon to get new video updates!!
-I am so glad to see new SUB :)
-歡迎來到Pan Piano 小P的音樂工房！
-這邊不定期分享動漫鋼琴演奏！歡迎訂閱與按下旁邊的鈴鐺：）
-官方網站 Offical Website：
-小P的音樂工房http://panpiano.com/ 
-～分享動漫鋼琴演奏與教學～</t>
-  </si>
-  <si>
-    <t>The official home of 2CELLOS - we post our new videos and live concert footage here every few weeks, so keep coming back for the latest 2CELLOS!!</t>
-  </si>
-  <si>
-    <t>久石譲のYouTube公式チャンネルです。Official YouTube channel of Joe Hisaishi.
-Joe Hisaishi—hailed by Pitchfork as “the most acclaimed Japanese composer to have ever worked in film”—has won countless awards for his achievements in composition and film scoring. He is the 8-time winner of the Japanese Academy Award for Best Music; he was awarded the Japan Medal of Honour award in 2009; and he has composed soundtracks for 2 Academy Award-winning films, “Departures” (2008) and “Spirited Away” (2002).
-Hisaishi’s body of work, comprised of nearly 100 film scores and solo albums, draws inspiration from the canon of American minimalist compositions, experimental electronic music, and European and Japanese classical music. He has scored all but one of Hayao Miyazaki’s Studio Ghibli films, including 3 of the top 5 highest-grossing anime films (worldwide).
-Hisaishi, the celebrated Japanese composer known for his beloved film scores and his work with acclaimed filmmakers Hayao
-運営：株式会社ワンダーシティ　©Wonder City Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First to Eleven, Andie Case &amp; Brooke Surgener are coming to Detroit, Chicago, and Cleveland at the end of April! Buy tickets here: www.linktree.com/firsttoeleven
-</t>
-  </si>
-  <si>
-    <t>元気です。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome to the official The Piano Guys YouTube channel! Paul, a Yamaha dealer who dabbled in videography, Jon, a professional pianist, Al, a music producer and studio engineer, and Steve, a cellist with a creative superpower called ADHD, all serendipitously joined forces to create the most successful YouTube instrumental music group in history. The Piano Guys’ mission is to inspire and spread hope through incomparably imaginative piano music videos filmed all over the world. On this channel you can regularly find piano covers of music from genres like top 40, pop, classic rock, R&amp;B, hip hop, country, and more. Make sure to subscribe and enable all post notifications. For instant updates, check out The Piano Guys via their social media accounts linked below.
-New music coming soon 🎹🎻
-Text us! (801) 217-9512 📱
-</t>
-  </si>
-  <si>
-    <t>Hi! 我是Eric周興哲,
-從前的我 喜歡練習獨立 和鋼琴說話
-現在的自己 
-把鋼琴和說話 變成一種溝通的方式...
-音樂 讓說話變得更自由</t>
-  </si>
-  <si>
-    <t>【美波 Official Youtube Channel】</t>
-  </si>
-  <si>
-    <t>兵庫県西宮出身のシンガーソングライター。_x000D_
-15年3月にタワレコ限定single「貴方解剖純愛歌～死ね～」でインディーズデビュー。_x000D_
-16年11月30日、ワーナーミュージック・ジャパン内レーベル unBORDE より1st single「生きていたんだよな」でメジャーデビュー。_x000D_
-17年9月に3枚のシングルを含む1st full album「青春のエキサイトメント」を発表。_x000D_
-8月に5th single「マリーゴールド」をリリース。年末には紅白歌合戦に初出演を果たす。_x000D_
-19年2月にセカンドフルアルバム「瞬間的シックスセンス」を発表。2月18日に初の単独日本武道館公演「AIMYON BUDOKAN -1995-」を開催する。_x000D_
-4月に「「映画クレヨンしんちゃん新婚旅行ハリケーン～失われたひろし～」主題歌を収録したシングル「ハルノヒ」をリリース。_x000D_
-5thシングル「マリーゴールド」が日本国内アーティストでは初の単曲でのストリーミング再生数1億回を突破した。
-7月にTBS系 火曜ドラマ「Heaven？～ご苦楽レストラン～」主題歌「真夏の夜の匂いがする」、10月に映画『空の青さを知る人よ』主題歌2曲を収録したシングル「空の青さを知る人よ」をリリース。_x000D_
-10月から20年の2月までホールとアリーナでの過去最大規模のワンマン・ツアー「AIMYON TOUR 2019 -SIXTH SENSE STORY-」を開催。全箇所即日ソールドアウト。12月には「Billboard 2019年年間TOP ARTISTS」を獲得、「オリコン年間ストリーミングランキング 2019」でも1位を記録し”2019年 1番聴かれたアーティスト”_x000D_
-となった。_x000D_
-日本テレビ「news zero」の1月からの新テーマ曲して書き下ろした楽曲、「さよならの今日に」を配信限定で2月14日にリリース。_x000D_
-4月からOA中の「ハルノヒ」と「マリーゴールド」が起用されたキリンの発泡酒「淡麗グリーンラベル」のTVCMに出演。_x000D_
-6月17日、TBS系 火曜ドラマ『私の家政夫ナギサさん』の主題歌で初のバラードシングル「裸の心」をリリース。_x000D_9月9日に3枚目のフルアルバム「おいしいパスタがあると聞いて」の発表する。</t>
-  </si>
-  <si>
-    <t>I’m RuRu, a piano youtuber from Taiwan.
+    <t>I’m RuRu, an ACG pianist from Taiwan.
 Making piano covers and sheets of Anime&amp;Game music.
 If you like my videos, please subscribe and share to your friends.♬
-台湾のピアノYoutuber ヾ(´︶`*)ﾉ♬
+台湾のACGピアニスト ヾ(´︶`*)ﾉ♬
 主にRuRuのアニソン、ゲーソンのピアノ演奏です～
 チャンネル登録とシェアをよろしくお願いします！
-來自台灣的鋼琴演奏Youtuber
+來自台灣的ACG鋼琴家
 主要音樂類型以動漫、電玩為主～
 歡迎訂閱及按下小鈴鐺 |･ω･)ﾉ
 🐤Join RuRu's Membership to support me create music videos
@@ -232,7 +122,11 @@
 🎹合作洽談/Business：rurupianomusic@gmail.com</t>
   </si>
   <si>
-    <t>シンガーソングライター、ボカロPのAyase、そしてAyaseがコンポーザーを務めるユニット・YOASOBIのYouTubeチャンネルです。</t>
+    <t>Hi 我是Eric周興哲
+從前的我 喜歡練習獨立 和鋼琴說話
+現在的自己 
+把鋼琴和說話 變成一種溝通的方式
+音樂 讓說話變得更自由</t>
   </si>
   <si>
     <t>音楽家・俳優・文筆家。
@@ -243,142 +137,269 @@
 11月からは「Gen Hoshino POP VIRUS World Tour」と題し、ワールド・ツアーの開催も決定。11月23日の上海での公演を皮切りに、ニューヨーク、横浜、台北の4都市で計5公演を行う。</t>
   </si>
   <si>
+    <t>毎週金曜19時更新!!音楽プロデューサー、ミュージシャンとして活動するコバソロが贈るエンターテイメントチャンネル!
+楽曲制作、タイアップ等も承っています。
+【コバソロ】
+　演奏、作詞作曲、編曲、撮影、動画作成、各デザインなどすべて自身で手がけるマルチクリエイター。
+「コバソロ」と検索すると自分しか出ないので名前がこれに決定。
+　ライブ、YOUTUBE動画などで活動中!
+無所属
+I live in Japan and I make music.Everything you see + hear on my page was produced and put together by me.
+Also - I absolutely love hearing feedback from you guys.. so please subscribe and leave a comment!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">台湾のピアニストです！ 
+アニソンを弾いてます～ 
+良かったら、チャンネル登録お願いします（ベルマークもクリックしましょう！）
+宜しくお願いいたします！
+キャラクターデザイン：深崎暮人(@misaki_cradle)
+Welcome to my channel~~
+I make piano covers of  Anime/GAME!
+Please subscribe to my channel and click the bell icon to get new video updates!!
+I am so glad to see new SUB :)
+The character is designed by Kurehito Misaki (@misaki_cradle)
+歡迎來到Pan Piano 小P的音樂工房！
+這邊不定期分享動漫鋼琴演奏！歡迎訂閱與按下旁邊的鈴鐺：）
+角色設計：深崎暮人(@misaki_cradle)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First to Eleven is cover band based out of Erie, PA - founded in 2009. They take your favorite songs and put a fun extra twist on them, with heavy guitar riffs, hard hitting drums, fun melodies, and even mashing up different styles from different songs. The band has an extensive and constantly growing catalogue of covers as well as major experience both live and in the studio.
+</t>
+  </si>
+  <si>
+    <t>兵庫県西宮出身のシンガーソングライター。_x000D_
+15年3月にタワレコ限定single「貴方解剖純愛歌～死ね～」でインディーズデビュー。_x000D_
+16年11月30日、ワーナーミュージック・ジャパン内レーベル unBORDE より1st single「生きていたんだよな」でメジャーデビュー。_x000D_
+17年9月に3枚のシングルを含む1st full album「青春のエキサイトメント」を発表。_x000D_
+8月に5th single「マリーゴールド」をリリース。年末には紅白歌合戦に初出演を果たす。_x000D_
+19年2月にセカンドフルアルバム「瞬間的シックスセンス」を発表。2月18日に初の単独日本武道館公演「AIMYON BUDOKAN -1995-」を開催する。_x000D_
+4月に「「映画クレヨンしんちゃん新婚旅行ハリケーン～失われたひろし～」主題歌を収録したシングル「ハルノヒ」をリリース。_x000D_
+5thシングル「マリーゴールド」が日本国内アーティストでは初の単曲でのストリーミング再生数1億回を突破した。
+7月にTBS系 火曜ドラマ「Heaven？～ご苦楽レストラン～」主題歌「真夏の夜の匂いがする」、10月に映画『空の青さを知る人よ』主題歌2曲を収録したシングル「空の青さを知る人よ」をリリース。_x000D_
+10月から20年の2月までホールとアリーナでの過去最大規模のワンマン・ツアー「AIMYON TOUR 2019 -SIXTH SENSE STORY-」を開催。全箇所即日ソールドアウト。12月には「Billboard 2019年年間TOP ARTISTS」を獲得、「オリコン年間ストリーミングランキング 2019」でも1位を記録し”2019年 1番聴かれたアーティスト”_x000D_
+となった。_x000D_
+日本テレビ「news zero」の1月からの新テーマ曲して書き下ろした楽曲、「さよならの今日に」を配信限定で2月14日にリリース。_x000D_
+4月からOA中の「ハルノヒ」と「マリーゴールド」が起用されたキリンの発泡酒「淡麗グリーンラベル」のTVCMに出演。_x000D_
+6月17日、TBS系 火曜ドラマ『私の家政夫ナギサさん』の主題歌で初のバラードシングル「裸の心」をリリース。_x000D_9月9日に3枚目のフルアルバム「おいしいパスタがあると聞いて」の発表する。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the official The Piano Guys YouTube channel! Paul, a Yamaha dealer who dabbled in videography, Jon, a professional pianist, Al, a music producer and studio engineer, and Steve, a cellist with a creative superpower called ADHD, all serendipitously joined forces to create the most successful YouTube instrumental music group in history. The Piano Guys’ mission is to inspire and spread hope through incomparably imaginative piano music videos filmed all over the world. On this channel you can regularly find piano covers of music from genres like top 40, pop, classic rock, R&amp;B, hip hop, country, and more. Make sure to subscribe and enable all post notifications. For instant updates, check out The Piano Guys via their social media accounts linked below.
+New music coming soon 🎹🎻
+Text us! (801) 217-9512 📱
+</t>
+  </si>
+  <si>
+    <t>元気です。</t>
+  </si>
+  <si>
+    <t>久石譲のYouTube公式チャンネルです。Official YouTube channel of Joe Hisaishi.
+Joe Hisaishi—hailed by Pitchfork as “the most acclaimed Japanese composer to have ever worked in film”—has won countless awards for his achievements in composition and film scoring. He is the 8-time winner of the Japanese Academy Award for Best Music; he was awarded the Japan Medal of Honour award in 2009; and he has composed soundtracks for 2 Academy Award-winning films, “Departures” (2008) and “Spirited Away” (2002).
+Hisaishi’s body of work, comprised of nearly 100 film scores and solo albums, draws inspiration from the canon of American minimalist compositions, experimental electronic music, and European and Japanese classical music. He has scored all but one of Hayao Miyazaki’s Studio Ghibli films, including 3 of the top 5 highest-grossing anime films (worldwide).
+Hisaishi, the celebrated Japanese composer known for his beloved film scores and his work with acclaimed filmmakers Hayao
+運営：株式会社ワンダーシティ　©Wonder City Inc.</t>
+  </si>
+  <si>
+    <t>シンガーソングライター、ボカロPのAyase、そしてAyaseがコンポーザーを務めるユニット・YOASOBIのYouTubeチャンネルです。</t>
+  </si>
+  <si>
+    <t>ヨルシカ / n-buna official channel</t>
+  </si>
+  <si>
+    <t>Jay Chou 周杰倫
+“New King of Asian Pop” — Time magazine (2003)
+“One of the most inﬂuential ﬁgures in Asia”— CNN (2009)
+Music Career
+-Iconic musician of the 21st century
+-Since his debut in 2000, he has composed, produced, released 14 studio albums, which sold over 30 million copies.
+-He holds the highest record sales for Asian male singer, and has won numerous music awards, including 15 GMAs (Chinese Grammy)
+Concerts
+-Accomplished 7 world tours, over 300 concerts, performed to more than 10 million people. Jay Chou is celebrating his two decades in the entertainment industry by launching his 20th Anniversary "Carnival " World Tour in Oct. 2019.</t>
+  </si>
+  <si>
+    <t>【美波 Official Youtube Channel】</t>
+  </si>
+  <si>
+    <t>A microphone and a white studio.
+And 1 rule. You’ve got 1 TAKE.
+＿
+Your Music.
+Your Everything.
+All in this one take.
+THE FIRST TAKE
+Less Filter, More Music.
+■「THE FIRST TAKE」OFFICIAL 
+Web Site: https://www.thefirsttake.jp/ 
+Instagram: https://www.instagram.com/the_firsttake/ 
+Twitter: https://twitter.com/The_FirstTake 
+TikTok: https://www.tiktok.com/@the_first_take 
+THE FIRST TIMES: https://www.thefirsttimes.jp/
+■RULES
+白いスタジオに置かれた一本のマイク。 
+ここでのルールはただ一つ。
+一発撮りのパフォーマンスをすること。 
+■STATEMENT
+ありのままの自分を。
+ありのままの音楽を。
+一度きりにこめる。
+THE FIRST TAKE
+ありのままの世界へ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The official home of 2CELLOS </t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
     <t>JP</t>
   </si>
   <si>
-    <t>TW</t>
+    <t>US</t>
   </si>
   <si>
     <t>HR</t>
   </si>
   <si>
-    <t>US</t>
+    <t>UUAYrMNl92jw6cpjdpBP8JyA</t>
+  </si>
+  <si>
+    <t>UU7S48XRADBqamQbgLxpBFcQ</t>
+  </si>
+  <si>
+    <t>UUPKlrgZXnnb89nSeITvTdGA</t>
+  </si>
+  <si>
+    <t>UUDbQblY1XASbgqOXmy6FOFQ</t>
+  </si>
+  <si>
+    <t>UUI7ktPB6toqucpkkCiolwLg</t>
+  </si>
+  <si>
+    <t>UUcE10s4MFy4eed7q7QkonZg</t>
+  </si>
+  <si>
+    <t>UUQVhrypJhw1HxuRV4gX6hoQ</t>
+  </si>
+  <si>
+    <t>UUmKurapML4BF9Bjtj4RbvXw</t>
+  </si>
+  <si>
+    <t>UUln9P4Qm3-EAY4aiEPmRwEA</t>
+  </si>
+  <si>
+    <t>UUxyzciBLt1Hyw06dlqwAIkw</t>
+  </si>
+  <si>
+    <t>UUvpredjG93ifbCP1Y77JyFA</t>
   </si>
   <si>
     <t>UURIgIJQWuBJ0Cv_VlU3USNA</t>
   </si>
   <si>
-    <t>UUDbQblY1XASbgqOXmy6FOFQ</t>
+    <t>UU8CU5nVhCQIdAGrFFp4loOQ</t>
+  </si>
+  <si>
+    <t>UU2JzylaIF8qeowc7-5VwwmA</t>
   </si>
   <si>
     <t>UU9zY_E8mcAo_Oq772LEZq8Q</t>
   </si>
   <si>
-    <t>UU8CU5nVhCQIdAGrFFp4loOQ</t>
-  </si>
-  <si>
-    <t>UUI7ktPB6toqucpkkCiolwLg</t>
-  </si>
-  <si>
     <t>UUyjuFsbclXyntSRMBAILzbw</t>
   </si>
   <si>
-    <t>UUxyzciBLt1Hyw06dlqwAIkw</t>
-  </si>
-  <si>
-    <t>UUcE10s4MFy4eed7q7QkonZg</t>
-  </si>
-  <si>
-    <t>UUln9P4Qm3-EAY4aiEPmRwEA</t>
-  </si>
-  <si>
-    <t>UUmKurapML4BF9Bjtj4RbvXw</t>
-  </si>
-  <si>
-    <t>UU7S48XRADBqamQbgLxpBFcQ</t>
-  </si>
-  <si>
-    <t>UU2JzylaIF8qeowc7-5VwwmA</t>
-  </si>
-  <si>
-    <t>UUQVhrypJhw1HxuRV4gX6hoQ</t>
-  </si>
-  <si>
-    <t>UUAYrMNl92jw6cpjdpBP8JyA</t>
-  </si>
-  <si>
-    <t>UUvpredjG93ifbCP1Y77JyFA</t>
-  </si>
-  <si>
-    <t>UUPKlrgZXnnb89nSeITvTdGA</t>
-  </si>
-  <si>
-    <t>['Music', 'Music_of_Asia', 'Pop_music', 'Independent_music', 'Rock_music']</t>
-  </si>
-  <si>
-    <t>['Pop_music', 'Music', 'Music_of_Asia']</t>
-  </si>
-  <si>
-    <t>['Classical_music', 'Music', 'Music_of_Asia']</t>
-  </si>
-  <si>
-    <t>['Music', 'Classical_music', 'Rock_music', 'Independent_music', 'Pop_music']</t>
-  </si>
-  <si>
-    <t>['Music', 'Classical_music']</t>
-  </si>
-  <si>
-    <t>['Pop_music', 'Music', 'Independent_music', 'Rock_music']</t>
-  </si>
-  <si>
-    <t>['Pop_music', 'Music', 'Electronic_music', 'Rock_music', 'Independent_music', 'Music_of_Asia']</t>
-  </si>
-  <si>
-    <t>['Pop_music', 'Music', 'Classical_music']</t>
-  </si>
-  <si>
-    <t>['Rock_music', 'Independent_music', 'Music', 'Pop_music', 'Music_of_Asia']</t>
-  </si>
-  <si>
-    <t>['Rock_music', 'Music_of_Asia', 'Pop_music', 'Music']</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_b_-qhgW9Ix681w7CVRpJmkqrciDIrCPb3fRjw=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu-9S3og5Ip2zFASnqMWKkjWatBfPT9ELeqUbTSL1A=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_bRdzxCJQzBxWFAz8Fr1StGZYQ0ApWSM93VZYgUg=s800-c-k-c0x00ffffff-no-rj</t>
+    <t>['Classical_music', 'Music_of_Asia', 'Music']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Music_of_Asia', 'Music']</t>
+  </si>
+  <si>
+    <t>['Lifestyle_(sociology)', 'Music_of_Asia', 'Classical_music', 'Music']</t>
+  </si>
+  <si>
+    <t>['Music', 'Pop_music', 'Rock_music']</t>
+  </si>
+  <si>
+    <t>['Music_of_Asia', 'Music', 'Rock_music', 'Pop_music']</t>
+  </si>
+  <si>
+    <t>['Classical_music', 'Pop_music', 'Music']</t>
+  </si>
+  <si>
+    <t>['Music_of_Asia', 'Music', 'Rock_music', 'Pop_music', 'Electronic_music']</t>
+  </si>
+  <si>
+    <t>['Classical_music', 'Music']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Music', 'Music_of_Asia', 'Entertainment']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Music_of_Asia', 'Rock_music', 'Music']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Music', 'Rock_music', 'Music_of_Asia']</t>
+  </si>
+  <si>
+    <t>['Classical_music', 'Pop_music', 'Rock_music', 'Music']</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AL5GRJV-W84rgttX8NZmqbEYYEwSh5vcACKEcpqR1rr9nKE=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/GFgkrFvg6tIF3XzfGJIb3q722cC-viI_SRplnNx3P5LWsGDtZlXTuxDOOG9WfZxWb1e-Iphy=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/7tQfJHMa8ZIi2HIDBNEqIrDTGK3kO8jRJgKSTpA99w8buRKoLugkegJ-WUDtn_zAQ_Mkd-6v_g=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AL5GRJUGPY9B7zPvrffjvHkyfoUnNxbszBIpGhyp5NhUBA=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AL5GRJX_2Ro7IwS7mm79yf29ixS3MRsDUl3e7-lri9deww=s800-c-k-c0x00ffffff-no-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/Xsyf4kJrHNMZl8ZJD-2wSWe_1Ob3s2hNFjQj0QCaJZjBXUZ40ORfoWgIilhxLEz_XR9NM7ogbg=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/sid2UtbKM4R3xfB0zIF7gpV3dCBUlc_yo3ohw-hCuax3_zEZh92IU1pf7CUUEk7mwKR5x2mAKGY=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/C8MtLsNIEqhl0DaXgIU_Y9dA8_ITbToxSmcpWKJJ0MTXo1GWJ4BjVEIqlc7OFQSzK6bRJY3CIA=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/I3ckNVLPQq04aQklOnRctTEnBjf7pkppVLV7WYe4Nb4g3sge1h-2IlXAvLnRGgrMkMfL4NadPQ=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/6pJyAmpgkwyRL5b3JCABfxOkfluyRw8wIaTS0cHMIGhOKr5dEmuquC9nsCxUl8Yp3KGQGavE-g=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AL5GRJVKazh6vCFxx-JhxshxN8JgRFW18RP11s9cHO_8Rw=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AL5GRJWLa7d3bmFC47nGIqrHrOIb5AvbpLVyZeyM7D0n=s800-c-k-c0x00ffffff-no-rj-mo</t>
   </si>
   <si>
     <t>https://yt3.ggpht.com/OvyupgLYH05byQQoYNw6BtXoCw1ygFYTMtGhk0vOTaOii8U9x5NYK1R4JD7FJAUCouqy_8JA=s800-c-k-c0x00ffffff-no-nd-rj</t>
   </si>
   <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu84_Satr9fc_VK7dmVjKI4EuIlXjazdzAAWpKUN2A=s800-c-k-c0x00ffffff-no-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu9V7gXnpIUCJYKKY_KANCGKI-0lrr0VeoRXYVce6A=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/6pJyAmpgkwyRL5b3JCABfxOkfluyRw8wIaTS0cHMIGhOKr5dEmuquC9nsCxUl8Yp3KGQGavE-g=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/Xsyf4kJrHNMZl8ZJD-2wSWe_1Ob3s2hNFjQj0QCaJZjBXUZ40ORfoWgIilhxLEz_XR9NM7ogbg=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/I3ckNVLPQq04aQklOnRctTEnBjf7pkppVLV7WYe4Nb4g3sge1h-2IlXAvLnRGgrMkMfL4NadPQ=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/VC8eWCWtSO-5LN-f-IQGDu8HfwmwoZaA9kuIwa7v-o0S0DX0YTVlNvgxErve31v5qeOF9jiSiw=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/GFgkrFvg6tIF3XzfGJIb3q722cC-viI_SRplnNx3P5LWsGDtZlXTuxDOOG9WfZxWb1e-Iphy=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu-a_zfDCmdvUihG0DgQdTY6aPT4lQ5Sst5qnvczgg=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/EuK-WoKwja8NatLUU0SfdSyxhDnlHRSV7tvtkWRDeYuNjsigu5vrMHyBAn5WVakHVWN_hICCvw=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu8rT2GCMKLVdsw7Usq8QxG7_OQ5nwkj3RKlqaP5TMg=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_8o8D8yLIaOLRZMOmVO0fS85nM-VlmWNJHQIJFLQ=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/DLCVX6ArRGaHMe4k4N7Q_QtYiSOwbJ0pHi9zNwegysTq2ozs3G3_CPxImF-2hh0E2SYVGOEc=s800-c-k-c0x00ffffff-no-nd-rj</t>
+    <t>https://yt3.ggpht.com/ytc/AL5GRJX3LQpbjmL1Vuoafmw7IuzmR6dsNcfTdQrwSYr1_A=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/P-EfSx-9Q-MSQCHVv7Dp9Cg8sV3LbLfc-a06hSWGcZ1n2q77nVUJqn51vBUhvbj_qIG73W66Ow=s800-c-k-c0x00ffffff-no-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AL5GRJUy1AO8MS_BbKtDpoOX0Rl2JjwsOvTjNtLTHiqKpQ=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>鋼琴 Ru味春捲 "Ru's Piano" "Ru Piano" Piano ピアノ "Anime Piano" "動漫 鋼琴" Pianist "Piano Cover" RUsPiano 鋼琴女神 "Cosplay Piano" "Cosplay 鋼琴" "ACG ピアノ" ピアノ</t>
+  </si>
+  <si>
+    <t>周興哲</t>
+  </si>
+  <si>
+    <t>星野源 ほしのげん ホシノゲン "Gen Hoshino" "Hoshino Gen" "星野 源"</t>
   </si>
   <si>
     <t>KOBASOLO コバソロ リトルタートルズ 音楽 music インディーズ little turtles live コバ カメ 癒し new 新宿 ストリート タワーレコード ＰＯＰ Ｒ＆Ｂ ＳＯＵＬ ビデオ</t>
@@ -387,28 +408,19 @@
     <t>鋼琴 演奏 ACG 動畫 漫畫 piano ピアノ アニメ 弾いてみた コスプレ パンピアノ "pan piano"</t>
   </si>
   <si>
+    <t>"first to eleven" "first to eleven youtube" "youtube first to eleven" f211 "f211 youtube" "youtube f211" female "female vocalist" "female singer" singing music artist "music artist" cover covers "cover band" band rock pop "pop rock" "rock cover" "pop cover" "pop rock cover"</t>
+  </si>
+  <si>
+    <t>thepianoguys "the piano guys" "piano guys" "piano guy" "piano guys youtube" "youtube piano guys" song music cover instrumental cello "cello song" "cello music" "cello cover" "cover cello" "cello instrumental" "instrumental cello" "cello performance" "cello live" "live cello" "cello songs" piano "piano song" "piano music" "piano cover" "cover piano" "piano instrumental" "instrumental piano" "piano performance" "live piano" "piano live" "piano songs" classical "classical music" "classical piano"</t>
+  </si>
+  <si>
+    <t>アド あぼ ado "アド 歌い手" ADO Ado "Ado TikTok" "アド ティックトック" "Ado 歌い手" 歌い手 "ado 邪魔" エーディーオー エイド うっせぇわ USSEEWA うっせぇわ 会いたくて 踊 レディメイド 夜のピエロ ギラギラ よくばり Ayase</t>
+  </si>
+  <si>
+    <t>シンガーソングライター</t>
+  </si>
+  <si>
     <t>2CELLOS Luka Sulic Stjepan Hauser Two Cellos</t>
-  </si>
-  <si>
-    <t>"first to eleven" "first to eleven youtube" "youtube first to eleven" f211 "f211 youtube" "youtube f211" female "female vocalist" "female singer" singing music artist "music artist" cover covers "cover band" band rock pop "pop rock" "rock cover" "pop cover" "pop rock cover"</t>
-  </si>
-  <si>
-    <t>アド あぼ ado "アド 歌い手" ADO Ado "Ado TikTok" "アド ティックトック" "Ado 歌い手" 歌い手 "ado 邪魔" エーディーオー エイド うっせぇわ USSEEWA うっせぇわ 会いたくて 踊 レディメイド 夜のピエロ ギラギラ よくばり Ayase</t>
-  </si>
-  <si>
-    <t>thepianoguys "the piano guys" "piano guys" "piano guy" "piano guys youtube" "youtube piano guys" song music cover instrumental cello "cello song" "cello music" "cello cover" "cover cello" "cello instrumental" "instrumental cello" "cello performance" "cello live" "live cello" "cello songs" piano "piano song" "piano music" "piano cover" "cover piano" "piano instrumental" "instrumental piano" "piano performance" "live piano" "piano live" "piano songs" classical "classical music" "classical piano"</t>
-  </si>
-  <si>
-    <t>周興哲</t>
-  </si>
-  <si>
-    <t>シンガーソングライター</t>
-  </si>
-  <si>
-    <t>鋼琴 Ru味春捲 "Ru's Piano" "Ru Piano" Piano ピアノ "Anime Piano" "動漫 鋼琴" Pianist "Piano Cover" RUsPiano 鋼琴女神 "Cosplay Piano" "Cosplay 鋼琴" "ACG ピアノ" ピアノ</t>
-  </si>
-  <si>
-    <t>星野源 ほしのげん ホシノゲン "Gen Hoshino" "Hoshino Gen" "星野 源"</t>
   </si>
 </sst>
 </file>
@@ -835,25 +847,31 @@
         <v>27</v>
       </c>
       <c r="D2" s="2">
-        <v>41355</v>
+        <v>43173</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
       </c>
       <c r="F2">
-        <v>2580000</v>
+        <v>2430000</v>
       </c>
       <c r="G2">
-        <v>1465894954</v>
+        <v>327306517</v>
       </c>
       <c r="H2" t="s">
         <v>47</v>
       </c>
       <c r="I2">
-        <v>51</v>
+        <v>480</v>
       </c>
       <c r="J2" t="s">
         <v>63</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="L2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -867,31 +885,31 @@
         <v>28</v>
       </c>
       <c r="D3" s="2">
-        <v>39629</v>
+        <v>41855</v>
       </c>
       <c r="E3" t="s">
         <v>43</v>
       </c>
       <c r="F3">
-        <v>3010000</v>
+        <v>1140000</v>
       </c>
       <c r="G3">
-        <v>1435937011</v>
+        <v>1388692215</v>
       </c>
       <c r="H3" t="s">
         <v>48</v>
       </c>
       <c r="I3">
-        <v>500</v>
+        <v>131</v>
       </c>
       <c r="J3" t="s">
         <v>64</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -905,28 +923,31 @@
         <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>43774</v>
+        <v>42132</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F4">
-        <v>6960000</v>
+        <v>1500000</v>
       </c>
       <c r="G4">
-        <v>2521573578</v>
+        <v>981417011</v>
       </c>
       <c r="H4" t="s">
         <v>49</v>
       </c>
       <c r="I4">
-        <v>449</v>
+        <v>123</v>
       </c>
       <c r="J4" t="s">
         <v>64</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -940,28 +961,31 @@
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>43767</v>
+        <v>39629</v>
       </c>
       <c r="E5" t="s">
         <v>44</v>
       </c>
       <c r="F5">
-        <v>2710000</v>
+        <v>3030000</v>
       </c>
       <c r="G5">
-        <v>3479411546</v>
+        <v>1472338939</v>
       </c>
       <c r="H5" t="s">
         <v>50</v>
       </c>
       <c r="I5">
-        <v>22</v>
+        <v>506</v>
       </c>
       <c r="J5" t="s">
         <v>64</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="L5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -978,28 +1002,28 @@
         <v>42578</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6">
-        <v>3430000</v>
+        <v>3470000</v>
       </c>
       <c r="G6">
-        <v>540223603</v>
+        <v>567634250</v>
       </c>
       <c r="H6" t="s">
         <v>51</v>
       </c>
       <c r="I6">
-        <v>566</v>
+        <v>647</v>
       </c>
       <c r="J6" t="s">
         <v>65</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1013,31 +1037,31 @@
         <v>32</v>
       </c>
       <c r="D7" s="2">
-        <v>40833</v>
+        <v>42346</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
       </c>
       <c r="F7">
-        <v>6320000</v>
+        <v>1550000</v>
       </c>
       <c r="G7">
-        <v>1633128098</v>
+        <v>471523907</v>
       </c>
       <c r="H7" t="s">
         <v>52</v>
       </c>
       <c r="I7">
-        <v>213</v>
+        <v>354</v>
       </c>
       <c r="J7" t="s">
         <v>66</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1051,28 +1075,28 @@
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>42762</v>
-      </c>
-      <c r="E8" t="s">
-        <v>43</v>
+        <v>41712</v>
       </c>
       <c r="F8">
-        <v>884000</v>
+        <v>1850000</v>
       </c>
       <c r="G8">
-        <v>141930811</v>
+        <v>1659790321</v>
       </c>
       <c r="H8" t="s">
         <v>53</v>
       </c>
       <c r="I8">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J8" t="s">
         <v>67</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1086,31 +1110,31 @@
         <v>34</v>
       </c>
       <c r="D9" s="2">
-        <v>42346</v>
+        <v>39532</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9">
-        <v>1470000</v>
+        <v>7070000</v>
       </c>
       <c r="G9">
-        <v>429229469</v>
+        <v>2275717411</v>
       </c>
       <c r="H9" t="s">
         <v>54</v>
       </c>
       <c r="I9">
-        <v>323</v>
+        <v>158</v>
       </c>
       <c r="J9" t="s">
         <v>68</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1127,28 +1151,28 @@
         <v>43330</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10">
-        <v>4370000</v>
+        <v>4870000</v>
       </c>
       <c r="G10">
-        <v>1625463501</v>
+        <v>1995100746</v>
       </c>
       <c r="H10" t="s">
         <v>55</v>
       </c>
       <c r="I10">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="J10" t="s">
         <v>69</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L10" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1162,31 +1186,28 @@
         <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>39532</v>
+        <v>42762</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F11">
-        <v>7030000</v>
+        <v>922000</v>
       </c>
       <c r="G11">
-        <v>2225527123</v>
+        <v>163124821</v>
       </c>
       <c r="H11" t="s">
         <v>56</v>
       </c>
       <c r="I11">
-        <v>153</v>
+        <v>65</v>
       </c>
       <c r="J11" t="s">
         <v>70</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="L11" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1200,31 +1221,28 @@
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>41855</v>
+        <v>43420</v>
       </c>
       <c r="E12" t="s">
         <v>44</v>
       </c>
       <c r="F12">
-        <v>1110000</v>
+        <v>4410000</v>
       </c>
       <c r="G12">
-        <v>1305973653</v>
+        <v>2426931476</v>
       </c>
       <c r="H12" t="s">
         <v>57</v>
       </c>
       <c r="I12">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L12" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1238,31 +1256,25 @@
         <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>42372</v>
-      </c>
-      <c r="E13" t="s">
-        <v>43</v>
+        <v>41355</v>
       </c>
       <c r="F13">
-        <v>1320000</v>
+        <v>2680000</v>
       </c>
       <c r="G13">
-        <v>423099409</v>
+        <v>1591759393</v>
       </c>
       <c r="H13" t="s">
         <v>58</v>
       </c>
       <c r="I13">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="J13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L13" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1276,28 +1288,28 @@
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>41712</v>
+        <v>43767</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
       </c>
       <c r="F14">
-        <v>1770000</v>
+        <v>2770000</v>
       </c>
       <c r="G14">
-        <v>1559078065</v>
+        <v>3678726272</v>
       </c>
       <c r="H14" t="s">
         <v>59</v>
       </c>
       <c r="I14">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="J14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L14" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1311,31 +1323,31 @@
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>43173</v>
+        <v>42372</v>
       </c>
       <c r="E15" t="s">
         <v>44</v>
       </c>
       <c r="F15">
-        <v>2350000</v>
+        <v>1350000</v>
       </c>
       <c r="G15">
-        <v>305496093</v>
+        <v>449748491</v>
       </c>
       <c r="H15" t="s">
         <v>60</v>
       </c>
       <c r="I15">
-        <v>413</v>
+        <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1349,28 +1361,28 @@
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>43420</v>
+        <v>43774</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16">
-        <v>4120000</v>
+        <v>7610000</v>
       </c>
       <c r="G16">
-        <v>2147163665</v>
+        <v>2909962689</v>
       </c>
       <c r="H16" t="s">
         <v>61</v>
       </c>
       <c r="I16">
-        <v>122</v>
+        <v>556</v>
       </c>
       <c r="J16" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1384,31 +1396,31 @@
         <v>42</v>
       </c>
       <c r="D17" s="2">
-        <v>42132</v>
+        <v>40833</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F17">
-        <v>1480000</v>
+        <v>6410000</v>
       </c>
       <c r="G17">
-        <v>939959835</v>
+        <v>1686010400</v>
       </c>
       <c r="H17" t="s">
         <v>62</v>
       </c>
       <c r="I17">
-        <v>99</v>
+        <v>213</v>
       </c>
       <c r="J17" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>